<commit_message>
df used for EDA
</commit_message>
<xml_diff>
--- a/data/disneydata/touringplans_data_dictionary.xlsx
+++ b/data/disneydata/touringplans_data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demetriusgreen/Dropbox/Stats_n_Programming/R Code/bigdataR_course/data/disneydata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D524D492-B33F-5247-9C81-76EE4D052180}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2DF280-DBE6-B04F-8323-22E9CCEAF509}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="11720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3151,8 +3151,8 @@
   <dimension ref="A1:D191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A163" sqref="A163:XFD163"/>
+      <pane ySplit="1" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6271,8 +6271,8 @@
   <dimension ref="A1:B80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>